<commit_message>
fixed small ratio calc bug
</commit_message>
<xml_diff>
--- a/data/Em3/Results.xlsx
+++ b/data/Em3/Results.xlsx
@@ -1113,13 +1113,13 @@
     <col min="40" max="40" width="22.7109375" customWidth="1"/>
     <col min="41" max="41" width="16.7109375" customWidth="1"/>
     <col min="42" max="42" width="9.7109375" customWidth="1"/>
-    <col min="43" max="43" width="19.7109375" customWidth="1"/>
+    <col min="43" max="43" width="20.7109375" customWidth="1"/>
     <col min="44" max="44" width="22.7109375" customWidth="1"/>
     <col min="45" max="45" width="22.7109375" customWidth="1"/>
     <col min="46" max="46" width="18.7109375" customWidth="1"/>
     <col min="47" max="47" width="9.7109375" customWidth="1"/>
     <col min="48" max="48" width="12.7109375" customWidth="1"/>
-    <col min="49" max="49" width="13.7109375" customWidth="1"/>
+    <col min="49" max="49" width="12.7109375" customWidth="1"/>
     <col min="50" max="50" width="20.7109375" customWidth="1"/>
     <col min="51" max="51" width="19.7109375" customWidth="1"/>
     <col min="52" max="52" width="12.7109375" customWidth="1"/>
@@ -1596,10 +1596,10 @@
         <v>32.7021</v>
       </c>
       <c r="AP3">
-        <v>0.1303</v>
+        <v>0.1301</v>
       </c>
       <c r="AQ3">
-        <v>0.3984453597781182</v>
+        <v>0.3978337782588885</v>
       </c>
       <c r="AR3">
         <v>0.0009971805842332693</v>
@@ -1617,13 +1617,13 @@
         <v>32.6481</v>
       </c>
       <c r="AW3">
-        <v>0.1308355836</v>
+        <v>0.132446191</v>
       </c>
       <c r="AX3">
         <v>0.1319051382045479</v>
       </c>
       <c r="AY3">
-        <v>0.4007448629476141</v>
+        <v>0.4056780976534622</v>
       </c>
       <c r="AZ3" t="s">
         <v>25</v>
@@ -1632,7 +1632,7 @@
         <v>510.3607669713487</v>
       </c>
       <c r="BC3">
-        <v>1.918411270035704</v>
+        <v>1.918640515037315</v>
       </c>
       <c r="BD3">
         <v>32590.1</v>
@@ -1672,7 +1672,7 @@
     <col min="13" max="13" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="18.7109375" customWidth="1"/>
     <col min="18" max="18" width="19.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
@@ -1831,19 +1831,19 @@
         <v>32.7021</v>
       </c>
       <c r="N3">
-        <v>0.1303</v>
+        <v>0.1301</v>
       </c>
       <c r="O3">
         <v>32.6481</v>
       </c>
       <c r="P3">
-        <v>0.1308355836</v>
+        <v>0.132446191</v>
       </c>
       <c r="Q3">
         <v>510.3607669713487</v>
       </c>
       <c r="R3">
-        <v>1.918411270035704</v>
+        <v>1.918640515037315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small correction to hydride table titles
</commit_message>
<xml_diff>
--- a/data/Em3/Results.xlsx
+++ b/data/Em3/Results.xlsx
@@ -1113,19 +1113,19 @@
     <col min="40" max="40" width="22.7109375" customWidth="1"/>
     <col min="41" max="41" width="16.7109375" customWidth="1"/>
     <col min="42" max="42" width="9.7109375" customWidth="1"/>
-    <col min="43" max="43" width="20.7109375" customWidth="1"/>
+    <col min="43" max="43" width="19.7109375" customWidth="1"/>
     <col min="44" max="44" width="22.7109375" customWidth="1"/>
     <col min="45" max="45" width="22.7109375" customWidth="1"/>
     <col min="46" max="46" width="18.7109375" customWidth="1"/>
     <col min="47" max="47" width="9.7109375" customWidth="1"/>
     <col min="48" max="48" width="12.7109375" customWidth="1"/>
-    <col min="49" max="49" width="12.7109375" customWidth="1"/>
+    <col min="49" max="49" width="13.7109375" customWidth="1"/>
     <col min="50" max="50" width="20.7109375" customWidth="1"/>
     <col min="51" max="51" width="19.7109375" customWidth="1"/>
     <col min="52" max="52" width="12.7109375" customWidth="1"/>
     <col min="53" max="53" width="6.7109375" customWidth="1"/>
     <col min="54" max="54" width="18.7109375" customWidth="1"/>
-    <col min="55" max="55" width="19.7109375" customWidth="1"/>
+    <col min="55" max="55" width="18.7109375" customWidth="1"/>
     <col min="56" max="56" width="11.7109375" customWidth="1"/>
     <col min="57" max="57" width="18.7109375" customWidth="1"/>
     <col min="58" max="58" width="19.7109375" customWidth="1"/>
@@ -1596,10 +1596,10 @@
         <v>32.7021</v>
       </c>
       <c r="AP3">
-        <v>0.1301</v>
+        <v>0.1286</v>
       </c>
       <c r="AQ3">
-        <v>0.3978337782588885</v>
+        <v>0.3932469168646662</v>
       </c>
       <c r="AR3">
         <v>0.0009971805842332693</v>
@@ -1617,13 +1617,13 @@
         <v>32.6481</v>
       </c>
       <c r="AW3">
-        <v>0.132446191</v>
+        <v>0.1323587271</v>
       </c>
       <c r="AX3">
         <v>0.1319051382045479</v>
       </c>
       <c r="AY3">
-        <v>0.4056780976534622</v>
+        <v>0.4054101987558234</v>
       </c>
       <c r="AZ3" t="s">
         <v>25</v>
@@ -1632,7 +1632,7 @@
         <v>510.3607669713487</v>
       </c>
       <c r="BC3">
-        <v>1.918640515037315</v>
+        <v>1.918627994592894</v>
       </c>
       <c r="BD3">
         <v>32590.1</v>
@@ -1672,9 +1672,9 @@
     <col min="13" max="13" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
     <col min="17" max="17" width="18.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1831,19 +1831,19 @@
         <v>32.7021</v>
       </c>
       <c r="N3">
-        <v>0.1301</v>
+        <v>0.1286</v>
       </c>
       <c r="O3">
         <v>32.6481</v>
       </c>
       <c r="P3">
-        <v>0.132446191</v>
+        <v>0.1323587271</v>
       </c>
       <c r="Q3">
         <v>510.3607669713487</v>
       </c>
       <c r="R3">
-        <v>1.918640515037315</v>
+        <v>1.918627994592894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added option to toggle fullscreen added different styles added github option
</commit_message>
<xml_diff>
--- a/data/Em3/Results.xlsx
+++ b/data/Em3/Results.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Calc" sheetId="2" r:id="rId2"/>
     <sheet name="Results" sheetId="3" r:id="rId3"/>
+    <sheet name="Constants" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="154">
   <si>
     <t>Lab. #</t>
   </si>
@@ -97,9 +98,6 @@
   </si>
   <si>
     <t>cryogenic cave calcite</t>
-  </si>
-  <si>
-    <t>044_018t8166.exp</t>
   </si>
   <si>
     <t>gem.</t>
@@ -460,6 +458,120 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>R34_33</t>
+  </si>
+  <si>
+    <t>R35_33</t>
+  </si>
+  <si>
+    <t>R30_29</t>
+  </si>
+  <si>
+    <t>mf48</t>
+  </si>
+  <si>
+    <t>mf36</t>
+  </si>
+  <si>
+    <t>mf56</t>
+  </si>
+  <si>
+    <t>mf68</t>
+  </si>
+  <si>
+    <t>mf92</t>
+  </si>
+  <si>
+    <t>mf38</t>
+  </si>
+  <si>
+    <t>mf35</t>
+  </si>
+  <si>
+    <t>mf43</t>
+  </si>
+  <si>
+    <t>mf45</t>
+  </si>
+  <si>
+    <t>mf09</t>
+  </si>
+  <si>
+    <t>mf29</t>
+  </si>
+  <si>
+    <t>mf34</t>
+  </si>
+  <si>
+    <t>mf58</t>
+  </si>
+  <si>
+    <t>mf02</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NR85</t>
+  </si>
+  <si>
+    <t>cps</t>
+  </si>
+  <si>
+    <t>slope229Correction</t>
+  </si>
+  <si>
+    <t>lambda232</t>
+  </si>
+  <si>
+    <t>lambda234</t>
+  </si>
+  <si>
+    <t>lambda238</t>
+  </si>
+  <si>
+    <t>lambda230</t>
+  </si>
+  <si>
+    <t>trisp236</t>
+  </si>
+  <si>
+    <t>trisp233</t>
+  </si>
+  <si>
+    <t>trisp229</t>
+  </si>
+  <si>
+    <t>blank234</t>
+  </si>
+  <si>
+    <t>blank234S</t>
+  </si>
+  <si>
+    <t>blank238</t>
+  </si>
+  <si>
+    <t>blank238S</t>
+  </si>
+  <si>
+    <t>blank232</t>
+  </si>
+  <si>
+    <t>blank232S</t>
+  </si>
+  <si>
+    <t>chBlank230</t>
+  </si>
+  <si>
+    <t>chBlank230S</t>
+  </si>
+  <si>
+    <t>a230232_init</t>
+  </si>
+  <si>
+    <t>a230232_init_err</t>
+  </si>
 </sst>
 </file>
 
@@ -482,20 +594,41 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDB310"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCDCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -515,9 +648,13 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -526,16 +663,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,7 +971,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -844,28 +984,27 @@
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
     <col min="20" max="20" width="19.7109375" customWidth="1"/>
     <col min="21" max="21" width="19.7109375" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" customWidth="1"/>
-    <col min="25" max="25" width="21.7109375" customWidth="1"/>
-    <col min="26" max="26" width="20.7109375" customWidth="1"/>
+    <col min="22" max="22" width="22.7109375" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" customWidth="1"/>
+    <col min="24" max="24" width="21.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:25" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,104 +1026,100 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="3" customFormat="1">
-      <c r="K2" s="3" t="s">
+    <row r="2" spans="1:25" s="2" customFormat="1">
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="V2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>8166</v>
       </c>
@@ -1000,61 +1135,58 @@
       <c r="G3">
         <v>0.1078</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
+      <c r="H3">
+        <v>0.009774971528730211</v>
       </c>
       <c r="I3">
-        <v>0.009774971528730211</v>
+        <v>1.030881597333003</v>
       </c>
       <c r="J3">
-        <v>1.030881597333003</v>
+        <v>0.007153779587876869</v>
       </c>
       <c r="K3">
-        <v>0.007153779587876869</v>
+        <v>0.02209471799659856</v>
       </c>
       <c r="L3">
-        <v>0.02209471799659856</v>
+        <v>3.125648482395934</v>
       </c>
       <c r="M3">
-        <v>3.125648482395934</v>
+        <v>0.01312080514307315</v>
       </c>
       <c r="N3">
-        <v>0.01312080514307315</v>
+        <v>3.546559926803768</v>
       </c>
       <c r="O3">
-        <v>3.546559926803768</v>
+        <v>1.081724026719631</v>
       </c>
       <c r="P3">
-        <v>1.081724026719631</v>
+        <v>0.01110677530290803</v>
       </c>
       <c r="Q3">
-        <v>0.01110677530290803</v>
+        <v>0.1188104752812409</v>
       </c>
       <c r="R3">
-        <v>0.1188104752812409</v>
+        <v>8.055334167077425E-05</v>
       </c>
       <c r="S3">
-        <v>8.055334167077425E-05</v>
+        <v>0.1188104752812417</v>
       </c>
       <c r="T3">
-        <v>0.1188104752812417</v>
+        <v>0.5832387890770165</v>
       </c>
       <c r="U3">
-        <v>0.5832387890770165</v>
+        <v>0.3212819427354254</v>
       </c>
       <c r="V3">
-        <v>0.3212819427354254</v>
+        <v>0.003553620086736945</v>
       </c>
       <c r="W3">
-        <v>0.003553620086736945</v>
+        <v>0.342231567409863</v>
       </c>
       <c r="X3">
-        <v>0.342231567409863</v>
+        <v>0.002070425876032709</v>
       </c>
       <c r="Y3">
-        <v>0.002070425876032709</v>
-      </c>
-      <c r="Z3">
         <v>0.2825407294232345</v>
       </c>
     </row>
@@ -1113,7 +1245,7 @@
     <col min="40" max="40" width="22.7109375" customWidth="1"/>
     <col min="41" max="41" width="16.7109375" customWidth="1"/>
     <col min="42" max="42" width="9.7109375" customWidth="1"/>
-    <col min="43" max="43" width="20.7109375" customWidth="1"/>
+    <col min="43" max="43" width="19.7109375" customWidth="1"/>
     <col min="44" max="44" width="22.7109375" customWidth="1"/>
     <col min="45" max="45" width="22.7109375" customWidth="1"/>
     <col min="46" max="46" width="18.7109375" customWidth="1"/>
@@ -1121,7 +1253,7 @@
     <col min="48" max="48" width="12.7109375" customWidth="1"/>
     <col min="49" max="49" width="13.7109375" customWidth="1"/>
     <col min="50" max="50" width="20.7109375" customWidth="1"/>
-    <col min="51" max="51" width="20.7109375" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" customWidth="1"/>
     <col min="52" max="52" width="12.7109375" customWidth="1"/>
     <col min="53" max="53" width="6.7109375" customWidth="1"/>
     <col min="54" max="54" width="18.7109375" customWidth="1"/>
@@ -1139,336 +1271,336 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="AF1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="AS1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BF1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:58" s="2" customFormat="1">
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:58" s="3" customFormat="1">
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="J2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="AR2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AS2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AN2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AW2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AU2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AY2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BA2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AY2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BD2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BB2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BE2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BE2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>29</v>
+      <c r="BF2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:58">
@@ -1596,10 +1728,10 @@
         <v>32.7021</v>
       </c>
       <c r="AP3">
-        <v>0.1294</v>
+        <v>0.1292</v>
       </c>
       <c r="AQ3">
-        <v>0.3956932429415848</v>
+        <v>0.3950816614223552</v>
       </c>
       <c r="AR3">
         <v>0.0009971805842332693</v>
@@ -1617,13 +1749,13 @@
         <v>32.6481</v>
       </c>
       <c r="AW3">
-        <v>0.1315954932</v>
+        <v>0.1319245405</v>
       </c>
       <c r="AX3">
         <v>0.1319051382045479</v>
       </c>
       <c r="AY3">
-        <v>0.4030724397438136</v>
+        <v>0.4040803002318664</v>
       </c>
       <c r="AZ3" t="s">
         <v>25</v>
@@ -1632,7 +1764,7 @@
         <v>510.3607669713487</v>
       </c>
       <c r="BC3">
-        <v>1.918519085318436</v>
+        <v>1.918565962079074</v>
       </c>
       <c r="BD3">
         <v>32590.1</v>
@@ -1686,108 +1818,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1">
-      <c r="C2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="3" t="s">
+    <row r="2" spans="1:19" s="2" customFormat="1">
+      <c r="C2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>102</v>
+      <c r="J2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1831,19 +1963,340 @@
         <v>32.7021</v>
       </c>
       <c r="N3">
-        <v>0.1294</v>
+        <v>0.1292</v>
       </c>
       <c r="O3">
         <v>32.6481</v>
       </c>
       <c r="P3">
-        <v>0.1315954932</v>
+        <v>0.1319245405</v>
       </c>
       <c r="Q3">
         <v>510.3607669713487</v>
       </c>
       <c r="R3">
-        <v>1.918519085318436</v>
+        <v>1.918565962079074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="4">
+        <v>0.002324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.005066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4.8E-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.336402435064349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.008202776684838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.334493224630051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.665506775369946</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.025840620457897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.673784240557133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.673784240557127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="4">
+        <v>-0.337307116990441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.336402435064353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="4">
+        <v>-0.34318587041139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="4">
+        <v>-1.025840620457897</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.337307116990439</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.682654750046506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6.02214129E+23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="4">
+        <v>137.881</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="4">
+        <v>62500000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3.4053</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4.94752E-11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2.82206E-06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1.55125E-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="4">
+        <v>9.1705E-06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3.86778</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.038556</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.018067</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>